<commit_message>
remove n from get_income
</commit_message>
<xml_diff>
--- a/database/industries/lastic/pekavir/product/monthly.xlsx
+++ b/database/industries/lastic/pekavir/product/monthly.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -693,7 +693,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BB61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AU4" workbookViewId="0">
+      <selection activeCell="BC31" sqref="BC31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2947,7 +2949,8 @@
         <v>3052</v>
       </c>
       <c r="AX24" s="11">
-        <v>3758756</v>
+        <f>3758756/1000</f>
+        <v>3758.7559999999999</v>
       </c>
       <c r="AY24" s="11">
         <v>2414</v>
@@ -4168,7 +4171,7 @@
         <v>3052</v>
       </c>
       <c r="AX33" s="17">
-        <v>3758756</v>
+        <v>3758.7559999999999</v>
       </c>
       <c r="AY33" s="17">
         <v>2414</v>

</xml_diff>

<commit_message>
complete pred income algorithm
</commit_message>
<xml_diff>
--- a/database/industries/lastic/pekavir/product/monthly.xlsx
+++ b/database/industries/lastic/pekavir/product/monthly.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Trade\database\industries\lastic\pekavir\product\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trade\database\industries\lastic\pekavir\product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95A19A3-2585-472E-AEF0-61F2749CAE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2655" yWindow="2655" windowWidth="17280" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -253,7 +252,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -725,17 +724,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BB61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="AU16" workbookViewId="0">
+      <selection activeCell="AX34" sqref="AX34:BB34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="54" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -790,7 +791,7 @@
       <c r="BA1" s="1"/>
       <c r="BB1" s="1"/>
     </row>
-    <row r="2" spans="2:54" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:54" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -847,7 +848,7 @@
       <c r="BA2" s="1"/>
       <c r="BB2" s="1"/>
     </row>
-    <row r="3" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -904,7 +905,7 @@
       <c r="BA3" s="1"/>
       <c r="BB3" s="1"/>
     </row>
-    <row r="4" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -959,7 +960,7 @@
       <c r="BA4" s="1"/>
       <c r="BB4" s="1"/>
     </row>
-    <row r="5" spans="2:54" ht="40.799999999999997" x14ac:dyDescent="0.75">
+    <row r="5" spans="2:54" ht="42" x14ac:dyDescent="0.65">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1016,7 +1017,7 @@
       <c r="BA5" s="4"/>
       <c r="BB5" s="4"/>
     </row>
-    <row r="6" spans="2:54" ht="40.799999999999997" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:54" ht="42" x14ac:dyDescent="0.65">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1073,7 +1074,7 @@
       <c r="BA6" s="4"/>
       <c r="BB6" s="4"/>
     </row>
-    <row r="7" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1128,7 +1129,7 @@
       <c r="BA7" s="1"/>
       <c r="BB7" s="1"/>
     </row>
-    <row r="8" spans="2:54" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -1285,7 +1286,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1340,7 +1341,7 @@
       <c r="BA9" s="1"/>
       <c r="BB9" s="1"/>
     </row>
-    <row r="10" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>4</v>
       </c>
@@ -1397,7 +1398,7 @@
       <c r="BA10" s="9"/>
       <c r="BB10" s="9"/>
     </row>
-    <row r="11" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>55</v>
       </c>
@@ -1556,7 +1557,7 @@
         <v>2656</v>
       </c>
     </row>
-    <row r="12" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
         <v>58</v>
       </c>
@@ -1715,7 +1716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>59</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
         <v>60</v>
       </c>
@@ -2033,7 +2034,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>61</v>
       </c>
@@ -2090,7 +2091,7 @@
       <c r="BA15" s="15"/>
       <c r="BB15" s="15"/>
     </row>
-    <row r="16" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B16" s="16" t="s">
         <v>62</v>
       </c>
@@ -2247,7 +2248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
         <v>63</v>
       </c>
@@ -2404,7 +2405,7 @@
         <v>2656</v>
       </c>
     </row>
-    <row r="18" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2459,7 +2460,7 @@
       <c r="BA18" s="1"/>
       <c r="BB18" s="1"/>
     </row>
-    <row r="19" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2514,7 +2515,7 @@
       <c r="BA19" s="1"/>
       <c r="BB19" s="1"/>
     </row>
-    <row r="20" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2569,7 +2570,7 @@
       <c r="BA20" s="1"/>
       <c r="BB20" s="1"/>
     </row>
-    <row r="21" spans="2:54" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>64</v>
       </c>
@@ -2726,7 +2727,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2781,7 +2782,7 @@
       <c r="BA22" s="1"/>
       <c r="BB22" s="1"/>
     </row>
-    <row r="23" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>64</v>
       </c>
@@ -2838,7 +2839,7 @@
       <c r="BA23" s="9"/>
       <c r="BB23" s="9"/>
     </row>
-    <row r="24" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
         <v>55</v>
       </c>
@@ -2982,7 +2983,8 @@
         <v>3052</v>
       </c>
       <c r="AX24" s="11">
-        <v>3758756</v>
+        <f>3758756/1000</f>
+        <v>3758.7559999999999</v>
       </c>
       <c r="AY24" s="11">
         <v>2414</v>
@@ -2997,7 +2999,7 @@
         <v>2455</v>
       </c>
     </row>
-    <row r="25" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
         <v>58</v>
       </c>
@@ -3156,7 +3158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
         <v>59</v>
       </c>
@@ -3315,7 +3317,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>60</v>
       </c>
@@ -3474,7 +3476,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
         <v>61</v>
       </c>
@@ -3531,7 +3533,7 @@
       <c r="BA28" s="15"/>
       <c r="BB28" s="15"/>
     </row>
-    <row r="29" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B29" s="16" t="s">
         <v>62</v>
       </c>
@@ -3688,7 +3690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
         <v>65</v>
       </c>
@@ -3745,7 +3747,7 @@
       <c r="BA30" s="9"/>
       <c r="BB30" s="9"/>
     </row>
-    <row r="31" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>55</v>
       </c>
@@ -3904,7 +3906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B32" s="18" t="s">
         <v>66</v>
       </c>
@@ -4061,7 +4063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B33" s="16" t="s">
         <v>63</v>
       </c>
@@ -4203,7 +4205,8 @@
         <v>3052</v>
       </c>
       <c r="AX33" s="17">
-        <v>3758756</v>
+        <f>3758756/1000</f>
+        <v>3758.7559999999999</v>
       </c>
       <c r="AY33" s="17">
         <v>2414</v>
@@ -4218,7 +4221,7 @@
         <v>2455</v>
       </c>
     </row>
-    <row r="34" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -4273,7 +4276,7 @@
       <c r="BA34" s="1"/>
       <c r="BB34" s="1"/>
     </row>
-    <row r="35" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -4328,7 +4331,7 @@
       <c r="BA35" s="1"/>
       <c r="BB35" s="1"/>
     </row>
-    <row r="36" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -4383,7 +4386,7 @@
       <c r="BA36" s="1"/>
       <c r="BB36" s="1"/>
     </row>
-    <row r="37" spans="2:54" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="s">
         <v>67</v>
       </c>
@@ -4540,7 +4543,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -4595,7 +4598,7 @@
       <c r="BA38" s="1"/>
       <c r="BB38" s="1"/>
     </row>
-    <row r="39" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
         <v>67</v>
       </c>
@@ -4652,7 +4655,7 @@
       <c r="BA39" s="9"/>
       <c r="BB39" s="9"/>
     </row>
-    <row r="40" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
         <v>55</v>
       </c>
@@ -4811,7 +4814,7 @@
         <v>2264156</v>
       </c>
     </row>
-    <row r="41" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B41" s="12" t="s">
         <v>58</v>
       </c>
@@ -4970,7 +4973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="s">
         <v>59</v>
       </c>
@@ -5129,7 +5132,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B43" s="12" t="s">
         <v>60</v>
       </c>
@@ -5288,7 +5291,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B44" s="14" t="s">
         <v>69</v>
       </c>
@@ -5345,7 +5348,7 @@
       <c r="BA44" s="15"/>
       <c r="BB44" s="15"/>
     </row>
-    <row r="45" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B45" s="16" t="s">
         <v>62</v>
       </c>
@@ -5504,7 +5507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
         <v>70</v>
       </c>
@@ -5561,7 +5564,7 @@
       <c r="BA46" s="9"/>
       <c r="BB46" s="9"/>
     </row>
-    <row r="47" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
         <v>55</v>
       </c>
@@ -5720,7 +5723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B48" s="18" t="s">
         <v>66</v>
       </c>
@@ -5879,7 +5882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="s">
         <v>71</v>
       </c>
@@ -5936,7 +5939,7 @@
       <c r="BA49" s="9"/>
       <c r="BB49" s="9"/>
     </row>
-    <row r="50" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
         <v>72</v>
       </c>
@@ -6095,7 +6098,7 @@
         <v>-2136</v>
       </c>
     </row>
-    <row r="51" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B51" s="18" t="s">
         <v>63</v>
       </c>
@@ -6252,7 +6255,7 @@
         <v>2262020</v>
       </c>
     </row>
-    <row r="52" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -6307,7 +6310,7 @@
       <c r="BA52" s="1"/>
       <c r="BB52" s="1"/>
     </row>
-    <row r="53" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -6362,7 +6365,7 @@
       <c r="BA53" s="1"/>
       <c r="BB53" s="1"/>
     </row>
-    <row r="54" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -6417,7 +6420,7 @@
       <c r="BA54" s="1"/>
       <c r="BB54" s="1"/>
     </row>
-    <row r="55" spans="2:54" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B55" s="7" t="s">
         <v>73</v>
       </c>
@@ -6574,7 +6577,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -6629,7 +6632,7 @@
       <c r="BA56" s="1"/>
       <c r="BB56" s="1"/>
     </row>
-    <row r="57" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B57" s="8" t="s">
         <v>74</v>
       </c>
@@ -6686,7 +6689,7 @@
       <c r="BA57" s="9"/>
       <c r="BB57" s="9"/>
     </row>
-    <row r="58" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>55</v>
       </c>
@@ -6845,7 +6848,7 @@
         <v>922409670</v>
       </c>
     </row>
-    <row r="59" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B59" s="12" t="s">
         <v>58</v>
       </c>
@@ -7004,7 +7007,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>59</v>
       </c>
@@ -7163,7 +7166,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B61" s="12" t="s">
         <v>60</v>
       </c>

</xml_diff>